<commit_message>
Add section about Excel and commas, and fix correlations calculation in Excel.
</commit_message>
<xml_diff>
--- a/static/BDC334/data/Correlation_data_env_calc.xlsx
+++ b/static/BDC334/data/Correlation_data_env_calc.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajsmit/Library/CloudStorage/Dropbox/R/workshops/R_courses/static/BDC334/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE2FB1D7-7143-7E4F-B22C-22855327E4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50B6E29-AB7D-BD42-BD47-61DD0FA8C2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6940" yWindow="4760" windowWidth="11160" windowHeight="10800" xr2:uid="{F914C9C1-7F9F-8B47-9B89-8604FF3520F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>site</t>
   </si>
@@ -427,7 +427,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,33 +546,21 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
-        <f>CORREL(B2:D2,B2:D2)</f>
+        <f>CORREL(B2:B8,B2:B8)</f>
         <v>1.0000000000000002</v>
       </c>
       <c r="C11" s="1"/>
@@ -584,15 +572,15 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1">
-        <f>CORREL(B2:D2,B3:D3)</f>
-        <v>-0.94491118252306827</v>
+        <f>CORREL(B2:B8,C2:C8)</f>
+        <v>-0.19142961929988561</v>
       </c>
       <c r="C12" s="1">
-        <f>CORREL(B3:D3,B3:D3)</f>
-        <v>1.0000000000000002</v>
+        <f>CORREL(C2:C8,C2:C8)</f>
+        <v>0.99999999999999989</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -602,26 +590,26 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1">
-        <f>CORREL(B2:D2,B4:D4)</f>
-        <v>-0.18898223650461363</v>
+        <f>CORREL(B2:B8,D2:D8)</f>
+        <v>-0.73607473809857782</v>
       </c>
       <c r="C13" s="1">
-        <f>CORREL(B3:D3,B4:D4)</f>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="D13" s="1"/>
+        <f>CORREL(C2:C8,D2:D8)</f>
+        <v>0.14537972933144117</v>
+      </c>
+      <c r="D13" s="1">
+        <f>CORREL(D2:D8,D2:D8)</f>
+        <v>1.0000000000000002</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -631,9 +619,6 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -643,9 +628,6 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -654,10 +636,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>

</xml_diff>